<commit_message>
updated xie with OR
</commit_message>
<xml_diff>
--- a/VA Xie JAMA paper/xie calculation.xlsx
+++ b/VA Xie JAMA paper/xie calculation.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\covid\VA Xie JAMA paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD8EDD3-EE74-4D02-9DA3-19FE2ED3A4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C46A39-2A45-4950-AEED-78624EFEB357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="3380" windowWidth="16270" windowHeight="13710" xr2:uid="{65B2E205-C6AE-4182-8F20-F511F927DFB7}"/>
+    <workbookView xWindow="7650" yWindow="2730" windowWidth="24050" windowHeight="18130" xr2:uid="{65B2E205-C6AE-4182-8F20-F511F927DFB7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Xie paper impact of vax" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>hospitalized for flu</t>
   </si>
@@ -83,9 +83,6 @@
     <t xml:space="preserve">to do the Fisher test, you look at control vs. experiment where </t>
   </si>
   <si>
-    <t>control = # flu unvaxxed , # of flu vaxxed in those hospitalized for COVID</t>
-  </si>
-  <si>
     <t>treatment = # flu unvaxxed , # of flu vaxxed in those hospitalized for FLU</t>
   </si>
   <si>
@@ -117,14 +114,58 @@
   </si>
   <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>flu vaccine</t>
+  </si>
+  <si>
+    <t># unvaxxed</t>
+  </si>
+  <si>
+    <t>control = # flu unvaxxed vs. # of flu vaxxed in those hospitalized for COVID</t>
+  </si>
+  <si>
+    <t># vaxxed</t>
+  </si>
+  <si>
+    <t>CONTROL (count for the opposite infection)</t>
+  </si>
+  <si>
+    <t>EXPERIMENT (count for this infection)</t>
+  </si>
+  <si>
+    <t>Intervention</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>Here are the  fisher values. OR &gt;1 means the vaccine mad thing worse.</t>
+  </si>
+  <si>
+    <t>COVID shot #1</t>
+  </si>
+  <si>
+    <t>COVID shot #2</t>
+  </si>
+  <si>
+    <t>COVID booster</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -152,14 +193,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -496,57 +539,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C6AEFE-8C4B-478A-8484-61153A9F5447}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.54296875" customWidth="1"/>
-    <col min="2" max="2" width="27.1796875" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
     <col min="3" max="3" width="27.1796875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2">
         <v>2403</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>8996</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -557,15 +602,15 @@
         <f>$B$2*B5/100</f>
         <v>453.92669999999998</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>20.73</v>
       </c>
-      <c r="E5" s="2">
-        <f>$D$2*D5/100</f>
+      <c r="F5" s="2">
+        <f>$E$2*E5/100</f>
         <v>1864.8708000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -576,15 +621,15 @@
         <f t="shared" ref="C6:C11" si="0">$B$2*B6/100</f>
         <v>113.90220000000001</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>4.2699999999999996</v>
       </c>
-      <c r="E6" s="2">
-        <f t="shared" ref="E6:E11" si="1">$D$2*D6/100</f>
+      <c r="F6" s="2">
+        <f>$E$2*E6/100</f>
         <v>384.12919999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -595,15 +640,15 @@
         <f t="shared" si="0"/>
         <v>516.88530000000003</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>20.46</v>
       </c>
-      <c r="E7" s="2">
-        <f t="shared" si="1"/>
+      <c r="F7" s="2">
+        <f>$E$2*E7/100</f>
         <v>1840.5816</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -614,20 +659,20 @@
         <f t="shared" si="0"/>
         <v>1318.0455000000002</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>54.54</v>
       </c>
-      <c r="E8" s="2">
-        <f t="shared" si="1"/>
+      <c r="F8" s="2">
+        <f>$E$2*E8/100</f>
         <v>4906.4183999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <f>100-B11</f>
@@ -637,18 +682,18 @@
         <f t="shared" si="0"/>
         <v>916.02359999999999</v>
       </c>
-      <c r="D10">
-        <f>100-D11</f>
+      <c r="E10">
+        <f>100-E11</f>
         <v>36.159999999999997</v>
       </c>
-      <c r="E10" s="2">
-        <f t="shared" si="1"/>
+      <c r="F10" s="2">
+        <f>$E$2*E10/100</f>
         <v>3252.9535999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>61.88</v>
@@ -657,32 +702,32 @@
         <f t="shared" si="0"/>
         <v>1486.9764000000002</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>63.84</v>
       </c>
-      <c r="E11" s="2">
-        <f t="shared" si="1"/>
+      <c r="F11" s="2">
+        <f>$E$2*E11/100</f>
         <v>5743.0464000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
@@ -707,42 +752,176 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="2">
+        <f>F10</f>
+        <v>3252.9535999999998</v>
+      </c>
+      <c r="C39" s="2">
+        <f>F11</f>
+        <v>5743.0464000000002</v>
+      </c>
+      <c r="E39" s="2">
+        <f>C10</f>
+        <v>916.02359999999999</v>
+      </c>
+      <c r="F39" s="2">
+        <f>C11</f>
+        <v>1486.9764000000002</v>
+      </c>
+      <c r="H39" s="1">
+        <f>F39/E39*B39/C39</f>
+        <v>0.91946024557721695</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="2">
+        <f>$C$5</f>
+        <v>453.92669999999998</v>
+      </c>
+      <c r="C40" s="2">
+        <f>C6</f>
+        <v>113.90220000000001</v>
+      </c>
+      <c r="E40" s="2">
+        <f>$F$5</f>
+        <v>1864.8708000000001</v>
+      </c>
+      <c r="F40" s="2">
+        <f>F6</f>
+        <v>384.12919999999997</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" ref="H40:H42" si="1">F40/E40*B40/C40</f>
+        <v>0.82088475293150198</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="2">
+        <f t="shared" ref="B41:B42" si="2">$C$5</f>
+        <v>453.92669999999998</v>
+      </c>
+      <c r="C41" s="2">
+        <f t="shared" ref="C41:C42" si="3">C7</f>
+        <v>516.88530000000003</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" ref="E41:E42" si="4">$F$5</f>
+        <v>1864.8708000000001</v>
+      </c>
+      <c r="F41" s="2">
+        <f t="shared" ref="F41:F42" si="5">F7</f>
+        <v>1840.5816</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" si="1"/>
+        <v>0.86675803197247459</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="2">
+        <f t="shared" si="2"/>
+        <v>453.92669999999998</v>
+      </c>
+      <c r="C42" s="2">
+        <f t="shared" si="3"/>
+        <v>1318.0455000000002</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="4"/>
+        <v>1864.8708000000001</v>
+      </c>
+      <c r="F42" s="2">
+        <f t="shared" si="5"/>
+        <v>4906.4183999999996</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="1"/>
+        <v>0.90608962477589805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>